<commit_message>
Lots of fixes and changes.
- Fixed the import command.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/celestials.xlsx
+++ b/resources/data-imports/Monsters/celestials.xlsx
@@ -418,8 +418,8 @@
   </sheetPr>
   <dimension ref="A1:AW30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO27" activeCellId="0" sqref="AO27:AO29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM32" activeCellId="0" sqref="AM32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>